<commit_message>
saveAs ist nun nur nach calculated klickbar
</commit_message>
<xml_diff>
--- a/examplets.xlsx
+++ b/examplets.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Artem</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>wert</t>
+  </si>
+  <si>
+    <t>//?page=1&amp;rows=2&amp;newname=$_otg&amp;cols=3,4&amp;val=5</t>
   </si>
 </sst>
 </file>
@@ -381,15 +384,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="49" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -405,8 +411,11 @@
       <c r="E1" t="s">
         <v>14</v>
       </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -423,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -440,7 +449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -457,7 +466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>

</xml_diff>